<commit_message>
Revisione dopo sal tecnico del 3 Giugno 2021
</commit_message>
<xml_diff>
--- a/900 - documenti/dwh_data_model_raccordo.xlsx
+++ b/900 - documenti/dwh_data_model_raccordo.xlsx
@@ -939,9 +939,6 @@
     <t>$char40.</t>
   </si>
   <si>
-    <t>cod_stato_asta</t>
-  </si>
-  <si>
     <t>dta_ultima_asta</t>
   </si>
   <si>
@@ -1222,6 +1219,9 @@
   </si>
   <si>
     <t>dta_estinzione</t>
+  </si>
+  <si>
+    <t>descr</t>
   </si>
 </sst>
 </file>
@@ -1640,10 +1640,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:Q334"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A151" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E166" sqref="E166"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N251" sqref="N251"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1720,7 +1721,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:17" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>74</v>
       </c>
@@ -1762,7 +1763,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:17" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>74</v>
       </c>
@@ -1794,7 +1795,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:17" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>74</v>
       </c>
@@ -1826,7 +1827,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:17" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>74</v>
       </c>
@@ -1858,7 +1859,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:17" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>74</v>
       </c>
@@ -1899,7 +1900,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:17" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>74</v>
       </c>
@@ -1940,7 +1941,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:17" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>74</v>
       </c>
@@ -1981,7 +1982,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:17" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>74</v>
       </c>
@@ -2022,7 +2023,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:17" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>74</v>
       </c>
@@ -2063,7 +2064,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="11" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:17" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>74</v>
       </c>
@@ -2104,7 +2105,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="12" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:17" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>74</v>
       </c>
@@ -2148,7 +2149,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="13" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:17" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>74</v>
       </c>
@@ -2190,7 +2191,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="14" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:17" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>74</v>
       </c>
@@ -2231,7 +2232,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="15" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:17" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>74</v>
       </c>
@@ -2263,7 +2264,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="16" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:17" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>74</v>
       </c>
@@ -2295,7 +2296,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="17" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>74</v>
       </c>
@@ -2327,7 +2328,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="18" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>74</v>
       </c>
@@ -2359,7 +2360,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="19" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>74</v>
       </c>
@@ -2391,7 +2392,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="20" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>74</v>
       </c>
@@ -2432,7 +2433,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="21" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>74</v>
       </c>
@@ -2464,7 +2465,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="22" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>74</v>
       </c>
@@ -2496,7 +2497,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="23" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>74</v>
       </c>
@@ -2528,7 +2529,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="24" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>74</v>
       </c>
@@ -2560,7 +2561,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="25" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>74</v>
       </c>
@@ -2602,7 +2603,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="26" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>74</v>
       </c>
@@ -2634,7 +2635,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="27" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>74</v>
       </c>
@@ -2666,7 +2667,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="28" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>74</v>
       </c>
@@ -2698,7 +2699,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="29" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>74</v>
       </c>
@@ -2739,7 +2740,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="30" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>74</v>
       </c>
@@ -2771,7 +2772,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="31" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>74</v>
       </c>
@@ -2812,7 +2813,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="32" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>74</v>
       </c>
@@ -2844,7 +2845,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="33" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>74</v>
       </c>
@@ -2876,7 +2877,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="34" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>74</v>
       </c>
@@ -2908,7 +2909,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="35" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>74</v>
       </c>
@@ -2940,7 +2941,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="36" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>74</v>
       </c>
@@ -2972,7 +2973,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="37" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>74</v>
       </c>
@@ -3004,7 +3005,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="38" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>74</v>
       </c>
@@ -3045,7 +3046,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="39" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>74</v>
       </c>
@@ -3086,7 +3087,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="40" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>74</v>
       </c>
@@ -3127,7 +3128,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="41" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>74</v>
       </c>
@@ -3168,7 +3169,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="42" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>74</v>
       </c>
@@ -3213,7 +3214,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="43" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>74</v>
       </c>
@@ -3254,7 +3255,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="44" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>74</v>
       </c>
@@ -3295,7 +3296,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="45" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>74</v>
       </c>
@@ -3336,7 +3337,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="46" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>74</v>
       </c>
@@ -3368,7 +3369,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="47" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>74</v>
       </c>
@@ -3409,7 +3410,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="48" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>74</v>
       </c>
@@ -3450,7 +3451,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="49" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>74</v>
       </c>
@@ -3491,7 +3492,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="50" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>74</v>
       </c>
@@ -3532,7 +3533,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="51" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>74</v>
       </c>
@@ -3573,7 +3574,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="52" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>74</v>
       </c>
@@ -3614,7 +3615,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="53" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>74</v>
       </c>
@@ -3655,7 +3656,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="54" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>74</v>
       </c>
@@ -3696,7 +3697,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="55" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>74</v>
       </c>
@@ -3716,7 +3717,7 @@
         <v>97</v>
       </c>
       <c r="G55" s="5" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="H55" s="1" t="s">
         <v>16</v>
@@ -3740,7 +3741,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="56" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>74</v>
       </c>
@@ -3781,7 +3782,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="57" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>74</v>
       </c>
@@ -3822,7 +3823,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="58" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>74</v>
       </c>
@@ -3866,7 +3867,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="59" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>74</v>
       </c>
@@ -3910,7 +3911,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="60" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>74</v>
       </c>
@@ -3951,7 +3952,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="61" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>74</v>
       </c>
@@ -3992,7 +3993,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="62" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>74</v>
       </c>
@@ -4036,7 +4037,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="63" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>74</v>
       </c>
@@ -4080,7 +4081,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="64" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>74</v>
       </c>
@@ -4121,7 +4122,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="65" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>74</v>
       </c>
@@ -4162,7 +4163,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="66" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>74</v>
       </c>
@@ -4203,7 +4204,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="67" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>74</v>
       </c>
@@ -4244,7 +4245,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="68" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>74</v>
       </c>
@@ -4285,7 +4286,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="69" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>74</v>
       </c>
@@ -4326,7 +4327,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="70" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>74</v>
       </c>
@@ -4346,7 +4347,7 @@
         <v>97</v>
       </c>
       <c r="G70" s="5" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="H70" s="1" t="s">
         <v>16</v>
@@ -4370,7 +4371,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="71" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>74</v>
       </c>
@@ -4414,7 +4415,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="72" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>74</v>
       </c>
@@ -4458,7 +4459,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="73" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>74</v>
       </c>
@@ -4499,7 +4500,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="74" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>74</v>
       </c>
@@ -4540,7 +4541,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="75" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>74</v>
       </c>
@@ -4581,7 +4582,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="76" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>74</v>
       </c>
@@ -4622,7 +4623,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="77" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>74</v>
       </c>
@@ -4666,7 +4667,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="78" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>74</v>
       </c>
@@ -4710,7 +4711,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="79" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>74</v>
       </c>
@@ -4751,7 +4752,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="80" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>74</v>
       </c>
@@ -4792,7 +4793,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="81" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>74</v>
       </c>
@@ -4833,7 +4834,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="82" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>74</v>
       </c>
@@ -4877,7 +4878,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="83" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>74</v>
       </c>
@@ -4918,7 +4919,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="84" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>74</v>
       </c>
@@ -4963,7 +4964,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="85" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>74</v>
       </c>
@@ -5008,7 +5009,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="86" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>74</v>
       </c>
@@ -5049,7 +5050,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="87" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>74</v>
       </c>
@@ -5069,7 +5070,7 @@
         <v>97</v>
       </c>
       <c r="G87" s="5" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="H87" s="1" t="s">
         <v>16</v>
@@ -5093,7 +5094,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="88" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>74</v>
       </c>
@@ -5134,7 +5135,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="89" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>74</v>
       </c>
@@ -5176,7 +5177,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="90" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>74</v>
       </c>
@@ -5217,7 +5218,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="91" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>74</v>
       </c>
@@ -5258,7 +5259,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="92" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>74</v>
       </c>
@@ -5302,7 +5303,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="93" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>74</v>
       </c>
@@ -5343,7 +5344,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="94" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>74</v>
       </c>
@@ -5385,7 +5386,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="95" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>74</v>
       </c>
@@ -5427,7 +5428,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="96" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>74</v>
       </c>
@@ -5472,7 +5473,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="97" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>74</v>
       </c>
@@ -5513,7 +5514,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="98" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>74</v>
       </c>
@@ -5554,7 +5555,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="99" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>74</v>
       </c>
@@ -5595,7 +5596,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="100" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>74</v>
       </c>
@@ -5637,7 +5638,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="101" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>74</v>
       </c>
@@ -5679,7 +5680,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="102" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
         <v>74</v>
       </c>
@@ -5721,7 +5722,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="103" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
         <v>74</v>
       </c>
@@ -5763,7 +5764,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="104" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
         <v>74</v>
       </c>
@@ -5805,7 +5806,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="105" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
         <v>74</v>
       </c>
@@ -5846,7 +5847,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="106" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
         <v>74</v>
       </c>
@@ -5878,7 +5879,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="107" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
         <v>74</v>
       </c>
@@ -5920,7 +5921,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="108" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
         <v>74</v>
       </c>
@@ -5962,7 +5963,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="109" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
         <v>74</v>
       </c>
@@ -6004,7 +6005,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="110" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
         <v>74</v>
       </c>
@@ -6046,7 +6047,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="111" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
         <v>74</v>
       </c>
@@ -6088,7 +6089,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="112" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
         <v>74</v>
       </c>
@@ -6130,7 +6131,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="113" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
         <v>74</v>
       </c>
@@ -6172,7 +6173,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="114" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
         <v>74</v>
       </c>
@@ -6217,7 +6218,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="115" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
         <v>74</v>
       </c>
@@ -6259,7 +6260,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="116" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
         <v>74</v>
       </c>
@@ -6301,7 +6302,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="117" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
         <v>74</v>
       </c>
@@ -6343,7 +6344,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="118" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
         <v>74</v>
       </c>
@@ -6385,7 +6386,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="119" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
         <v>74</v>
       </c>
@@ -6426,7 +6427,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="120" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
         <v>74</v>
       </c>
@@ -6467,7 +6468,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="121" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
         <v>74</v>
       </c>
@@ -6508,7 +6509,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="122" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
         <v>74</v>
       </c>
@@ -6549,7 +6550,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="123" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
         <v>74</v>
       </c>
@@ -6590,7 +6591,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="124" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
         <v>74</v>
       </c>
@@ -6631,7 +6632,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="125" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
         <v>74</v>
       </c>
@@ -6672,7 +6673,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="126" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
         <v>74</v>
       </c>
@@ -6713,7 +6714,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="127" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
         <v>74</v>
       </c>
@@ -6754,7 +6755,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="128" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
         <v>74</v>
       </c>
@@ -6795,7 +6796,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="129" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
         <v>74</v>
       </c>
@@ -6836,7 +6837,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="130" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
         <v>74</v>
       </c>
@@ -6856,7 +6857,7 @@
         <v>97</v>
       </c>
       <c r="G130" s="5" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="H130" s="1" t="s">
         <v>16</v>
@@ -6880,7 +6881,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="131" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
         <v>74</v>
       </c>
@@ -6921,7 +6922,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="132" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
         <v>74</v>
       </c>
@@ -6962,7 +6963,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="133" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
         <v>74</v>
       </c>
@@ -7003,7 +7004,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="134" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
         <v>74</v>
       </c>
@@ -7044,7 +7045,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="135" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
         <v>74</v>
       </c>
@@ -7076,7 +7077,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="136" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
         <v>74</v>
       </c>
@@ -7117,7 +7118,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="137" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
         <v>74</v>
       </c>
@@ -7158,7 +7159,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="138" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
         <v>74</v>
       </c>
@@ -7199,7 +7200,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="139" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
         <v>74</v>
       </c>
@@ -7240,7 +7241,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="140" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
         <v>74</v>
       </c>
@@ -7281,7 +7282,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="141" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
         <v>74</v>
       </c>
@@ -7322,7 +7323,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="142" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
         <v>74</v>
       </c>
@@ -7363,7 +7364,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="143" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
         <v>74</v>
       </c>
@@ -7404,7 +7405,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="144" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
         <v>74</v>
       </c>
@@ -7445,7 +7446,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="145" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:17" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
         <v>74</v>
       </c>
@@ -7487,7 +7488,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="146" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:17" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
         <v>74</v>
       </c>
@@ -7528,7 +7529,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="147" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:17" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
         <v>74</v>
       </c>
@@ -7569,7 +7570,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="148" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:17" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
         <v>74</v>
       </c>
@@ -7610,7 +7611,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="149" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:17" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
         <v>74</v>
       </c>
@@ -7630,7 +7631,7 @@
         <v>97</v>
       </c>
       <c r="G149" s="5" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="H149" s="1" t="s">
         <v>16</v>
@@ -7654,7 +7655,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="150" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:17" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
         <v>74</v>
       </c>
@@ -7695,7 +7696,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="151" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:17" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
         <v>74</v>
       </c>
@@ -7736,7 +7737,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="152" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:17" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
         <v>74</v>
       </c>
@@ -7778,10 +7779,10 @@
         <v>21946</v>
       </c>
       <c r="Q152" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="153" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="153" spans="1:17" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
         <v>74</v>
       </c>
@@ -7792,13 +7793,13 @@
         <v>14</v>
       </c>
       <c r="D153" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="E153" t="s">
         <v>15</v>
       </c>
       <c r="F153" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="H153" t="s">
         <v>19</v>
@@ -7823,10 +7824,10 @@
         <v>401768</v>
       </c>
       <c r="Q153" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="154" spans="1:17" x14ac:dyDescent="0.35">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="154" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
         <v>74</v>
       </c>
@@ -7867,7 +7868,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="155" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:17" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
         <v>74</v>
       </c>
@@ -7908,7 +7909,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="156" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:17" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
         <v>74</v>
       </c>
@@ -7949,7 +7950,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="157" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:17" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
         <v>74</v>
       </c>
@@ -7990,7 +7991,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="158" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:17" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
         <v>74</v>
       </c>
@@ -8031,7 +8032,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="159" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:17" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
         <v>74</v>
       </c>
@@ -8072,7 +8073,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="160" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:17" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
         <v>74</v>
       </c>
@@ -8113,7 +8114,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="161" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:17" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
         <v>74</v>
       </c>
@@ -8154,10 +8155,10 @@
         <v>21946</v>
       </c>
       <c r="Q161" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="162" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="162" spans="1:17" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
         <v>74</v>
       </c>
@@ -8168,7 +8169,7 @@
         <v>22</v>
       </c>
       <c r="D162" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="E162" t="s">
         <v>15</v>
@@ -8198,10 +8199,10 @@
         <v>401768</v>
       </c>
       <c r="Q162" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="163" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="163" spans="1:17" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
         <v>74</v>
       </c>
@@ -8242,7 +8243,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="164" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:17" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
         <v>74</v>
       </c>
@@ -8283,7 +8284,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="165" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:17" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
         <v>74</v>
       </c>
@@ -8324,10 +8325,10 @@
         <v>21946</v>
       </c>
       <c r="Q165" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="166" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="166" spans="1:17" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
         <v>74</v>
       </c>
@@ -8338,7 +8339,7 @@
         <v>25</v>
       </c>
       <c r="D166" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="E166" t="s">
         <v>15</v>
@@ -8368,10 +8369,10 @@
         <v>401768</v>
       </c>
       <c r="Q166" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="167" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="167" spans="1:17" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
         <v>74</v>
       </c>
@@ -8412,10 +8413,10 @@
         <v>21946</v>
       </c>
       <c r="Q167" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="168" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="168" spans="1:17" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
         <v>74</v>
       </c>
@@ -8426,7 +8427,7 @@
         <v>27</v>
       </c>
       <c r="D168" s="11" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="E168" t="s">
         <v>15</v>
@@ -8456,10 +8457,10 @@
         <v>401768</v>
       </c>
       <c r="Q168" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="169" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="169" spans="1:17" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
         <v>74</v>
       </c>
@@ -8470,13 +8471,13 @@
         <v>28</v>
       </c>
       <c r="D169" t="s">
+        <v>398</v>
+      </c>
+      <c r="E169" t="s">
+        <v>15</v>
+      </c>
+      <c r="F169" t="s">
         <v>399</v>
-      </c>
-      <c r="E169" t="s">
-        <v>15</v>
-      </c>
-      <c r="F169" t="s">
-        <v>400</v>
       </c>
       <c r="H169" t="s">
         <v>16</v>
@@ -8500,7 +8501,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="170" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
         <v>74</v>
       </c>
@@ -8541,7 +8542,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="171" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:17" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
         <v>74</v>
       </c>
@@ -8582,7 +8583,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="172" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:17" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
         <v>74</v>
       </c>
@@ -8623,7 +8624,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="173" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:17" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
         <v>74</v>
       </c>
@@ -8664,10 +8665,10 @@
         <v>21946</v>
       </c>
       <c r="Q173" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="174" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="174" spans="1:17" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
         <v>74</v>
       </c>
@@ -8678,7 +8679,7 @@
         <v>4</v>
       </c>
       <c r="D174" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="E174" t="s">
         <v>15</v>
@@ -8708,10 +8709,10 @@
         <v>401768</v>
       </c>
       <c r="Q174" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="175" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="175" spans="1:17" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
         <v>74</v>
       </c>
@@ -8731,7 +8732,7 @@
         <v>97</v>
       </c>
       <c r="G175" s="5" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="H175" s="1" t="s">
         <v>16</v>
@@ -8755,7 +8756,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="176" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:17" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
         <v>74</v>
       </c>
@@ -8796,10 +8797,10 @@
         <v>21946</v>
       </c>
       <c r="Q176" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="177" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="177" spans="1:17" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
         <v>74</v>
       </c>
@@ -8810,7 +8811,7 @@
         <v>6</v>
       </c>
       <c r="D177" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="E177" t="s">
         <v>15</v>
@@ -8840,10 +8841,10 @@
         <v>401768</v>
       </c>
       <c r="Q177" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="178" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="178" spans="1:17" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
         <v>74</v>
       </c>
@@ -8884,7 +8885,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="179" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:17" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
         <v>74</v>
       </c>
@@ -8926,7 +8927,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="180" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:17" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A180" t="s">
         <v>74</v>
       </c>
@@ -8968,7 +8969,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="181" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:17" hidden="1" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
         <v>74</v>
       </c>
@@ -9009,7 +9010,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="182" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:17" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
         <v>74</v>
       </c>
@@ -9050,7 +9051,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="183" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:17" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A183" t="s">
         <v>74</v>
       </c>
@@ -9091,7 +9092,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="184" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:17" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A184" t="s">
         <v>74</v>
       </c>
@@ -9132,7 +9133,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="185" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:17" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A185" t="s">
         <v>74</v>
       </c>
@@ -9173,7 +9174,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="186" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:17" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A186" t="s">
         <v>74</v>
       </c>
@@ -9214,7 +9215,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="187" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:17" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A187" t="s">
         <v>74</v>
       </c>
@@ -9255,7 +9256,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="188" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:17" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A188" t="s">
         <v>74</v>
       </c>
@@ -9275,7 +9276,7 @@
         <v>97</v>
       </c>
       <c r="G188" s="5" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="H188" s="1" t="s">
         <v>16</v>
@@ -9299,7 +9300,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="189" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:17" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A189" t="s">
         <v>74</v>
       </c>
@@ -9310,7 +9311,7 @@
         <v>9</v>
       </c>
       <c r="D189" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="E189" t="s">
         <v>15</v>
@@ -9340,7 +9341,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="190" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:17" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A190" t="s">
         <v>74</v>
       </c>
@@ -9381,7 +9382,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="191" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:17" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A191" t="s">
         <v>74</v>
       </c>
@@ -9422,7 +9423,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="192" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:17" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A192" t="s">
         <v>74</v>
       </c>
@@ -9463,7 +9464,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="193" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A193" t="s">
         <v>74</v>
       </c>
@@ -9504,7 +9505,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="194" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A194" t="s">
         <v>74</v>
       </c>
@@ -9545,7 +9546,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="195" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A195" t="s">
         <v>74</v>
       </c>
@@ -9586,7 +9587,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="196" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A196" t="s">
         <v>74</v>
       </c>
@@ -9627,7 +9628,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="197" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A197" t="s">
         <v>74</v>
       </c>
@@ -9668,7 +9669,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="198" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A198" t="s">
         <v>74</v>
       </c>
@@ -9679,7 +9680,7 @@
         <v>18</v>
       </c>
       <c r="D198" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="E198" t="s">
         <v>15</v>
@@ -9709,7 +9710,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="199" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A199" t="s">
         <v>74</v>
       </c>
@@ -9750,7 +9751,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="200" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A200" t="s">
         <v>74</v>
       </c>
@@ -9791,7 +9792,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="201" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A201" t="s">
         <v>74</v>
       </c>
@@ -9832,7 +9833,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="202" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A202" t="s">
         <v>74</v>
       </c>
@@ -9843,7 +9844,7 @@
         <v>22</v>
       </c>
       <c r="D202" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="E202" t="s">
         <v>15</v>
@@ -9873,7 +9874,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="203" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A203" t="s">
         <v>74</v>
       </c>
@@ -9914,7 +9915,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="204" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A204" t="s">
         <v>74</v>
       </c>
@@ -9955,7 +9956,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="205" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A205" t="s">
         <v>74</v>
       </c>
@@ -9996,7 +9997,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="206" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A206" t="s">
         <v>74</v>
       </c>
@@ -10037,7 +10038,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="207" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A207" t="s">
         <v>74</v>
       </c>
@@ -10078,7 +10079,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="208" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A208" t="s">
         <v>74</v>
       </c>
@@ -10120,7 +10121,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="209" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A209" t="s">
         <v>74</v>
       </c>
@@ -10162,7 +10163,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="210" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A210" t="s">
         <v>74</v>
       </c>
@@ -10204,7 +10205,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="211" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A211" t="s">
         <v>74</v>
       </c>
@@ -10245,7 +10246,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="212" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A212" t="s">
         <v>74</v>
       </c>
@@ -10286,7 +10287,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="213" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A213" t="s">
         <v>74</v>
       </c>
@@ -10327,7 +10328,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="214" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A214" t="s">
         <v>74</v>
       </c>
@@ -10368,7 +10369,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="215" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A215" t="s">
         <v>74</v>
       </c>
@@ -10388,7 +10389,7 @@
         <v>97</v>
       </c>
       <c r="G215" s="5" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="H215" s="1" t="s">
         <v>16</v>
@@ -10412,7 +10413,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="216" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A216" t="s">
         <v>74</v>
       </c>
@@ -10453,7 +10454,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="217" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A217" t="s">
         <v>74</v>
       </c>
@@ -10495,7 +10496,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="218" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A218" t="s">
         <v>74</v>
       </c>
@@ -10537,7 +10538,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="219" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A219" t="s">
         <v>74</v>
       </c>
@@ -10578,7 +10579,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="220" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A220" t="s">
         <v>74</v>
       </c>
@@ -10619,7 +10620,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="221" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A221" t="s">
         <v>74</v>
       </c>
@@ -10660,7 +10661,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="222" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A222" t="s">
         <v>74</v>
       </c>
@@ -10680,7 +10681,7 @@
         <v>97</v>
       </c>
       <c r="G222" s="5" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="H222" s="1" t="s">
         <v>16</v>
@@ -10704,7 +10705,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="223" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A223" t="s">
         <v>74</v>
       </c>
@@ -10745,7 +10746,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="224" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A224" t="s">
         <v>74</v>
       </c>
@@ -10787,7 +10788,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="225" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A225" t="s">
         <v>74</v>
       </c>
@@ -10828,7 +10829,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="226" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A226" t="s">
         <v>74</v>
       </c>
@@ -10869,7 +10870,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="227" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A227" t="s">
         <v>74</v>
       </c>
@@ -10910,7 +10911,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="228" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A228" t="s">
         <v>74</v>
       </c>
@@ -10930,7 +10931,7 @@
         <v>97</v>
       </c>
       <c r="G228" s="5" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="H228" s="1" t="s">
         <v>16</v>
@@ -10954,7 +10955,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="229" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A229" t="s">
         <v>74</v>
       </c>
@@ -10995,7 +10996,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="230" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A230" t="s">
         <v>74</v>
       </c>
@@ -11036,7 +11037,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="231" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A231" t="s">
         <v>74</v>
       </c>
@@ -11077,7 +11078,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="232" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="232" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A232" t="s">
         <v>74</v>
       </c>
@@ -11097,7 +11098,7 @@
         <v>97</v>
       </c>
       <c r="G232" s="5" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="H232" s="1" t="s">
         <v>16</v>
@@ -11121,7 +11122,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="233" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="233" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A233" t="s">
         <v>74</v>
       </c>
@@ -11162,7 +11163,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="234" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="234" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A234" t="s">
         <v>74</v>
       </c>
@@ -11203,7 +11204,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="235" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="235" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A235" t="s">
         <v>74</v>
       </c>
@@ -11245,7 +11246,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="236" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="236" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A236" t="s">
         <v>74</v>
       </c>
@@ -11286,7 +11287,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="237" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="237" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A237" t="s">
         <v>74</v>
       </c>
@@ -11327,7 +11328,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="238" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="238" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A238" t="s">
         <v>74</v>
       </c>
@@ -11368,7 +11369,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="239" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="239" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A239" t="s">
         <v>74</v>
       </c>
@@ -11409,7 +11410,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="240" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="240" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A240" t="s">
         <v>74</v>
       </c>
@@ -11429,7 +11430,7 @@
         <v>97</v>
       </c>
       <c r="G240" s="5" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="H240" s="1" t="s">
         <v>16</v>
@@ -11453,7 +11454,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="241" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="241" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A241" t="s">
         <v>74</v>
       </c>
@@ -11494,7 +11495,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="242" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="242" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A242" t="s">
         <v>74</v>
       </c>
@@ -11535,7 +11536,7 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="243" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="243" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A243" t="s">
         <v>74</v>
       </c>
@@ -11920,19 +11921,19 @@
         <v>15</v>
       </c>
       <c r="F251" s="5" t="s">
-        <v>306</v>
+        <v>214</v>
       </c>
       <c r="G251" s="5" t="s">
-        <v>303</v>
+        <v>400</v>
       </c>
       <c r="H251" s="5" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="I251" s="2">
-        <v>8</v>
+        <v>255</v>
       </c>
       <c r="J251" s="5" t="s">
-        <v>85</v>
+        <v>388</v>
       </c>
       <c r="K251" s="5" t="s">
         <v>19</v>
@@ -11940,13 +11941,10 @@
       <c r="L251" s="2">
         <v>255</v>
       </c>
-      <c r="M251" s="5" t="str">
-        <f t="shared" si="16"/>
-        <v>8.</v>
-      </c>
-      <c r="N251" s="1" t="s">
-        <v>102</v>
-      </c>
+      <c r="M251" s="5" t="s">
+        <v>388</v>
+      </c>
+      <c r="N251" s="1"/>
       <c r="O251" s="3">
         <v>43831</v>
       </c>
@@ -11971,10 +11969,10 @@
         <v>15</v>
       </c>
       <c r="F252" t="s">
+        <v>306</v>
+      </c>
+      <c r="G252" s="5" t="s">
         <v>307</v>
-      </c>
-      <c r="G252" s="5" t="s">
-        <v>308</v>
       </c>
       <c r="H252" s="5" t="s">
         <v>16</v>
@@ -12019,10 +12017,10 @@
         <v>15</v>
       </c>
       <c r="F253" t="s">
+        <v>308</v>
+      </c>
+      <c r="G253" s="5" t="s">
         <v>309</v>
-      </c>
-      <c r="G253" s="5" t="s">
-        <v>310</v>
       </c>
       <c r="H253" s="5" t="s">
         <v>16</v>
@@ -12067,10 +12065,10 @@
         <v>15</v>
       </c>
       <c r="F254" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="G254" s="5" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="H254" s="5" t="s">
         <v>16</v>
@@ -12115,10 +12113,10 @@
         <v>15</v>
       </c>
       <c r="F255" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="G255" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="H255" s="5" t="s">
         <v>16</v>
@@ -12163,10 +12161,10 @@
         <v>15</v>
       </c>
       <c r="F256" s="5" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="G256" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="H256" s="5" t="s">
         <v>16</v>
@@ -12205,13 +12203,13 @@
         <v>14</v>
       </c>
       <c r="D257" s="5" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="E257" s="10" t="s">
         <v>15</v>
       </c>
       <c r="F257" s="5" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="H257" s="5" t="s">
         <v>16</v>
@@ -12268,7 +12266,7 @@
         <v>255</v>
       </c>
       <c r="J258" s="5" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="K258" s="5" t="s">
         <v>19</v>
@@ -12351,7 +12349,7 @@
         <v>97</v>
       </c>
       <c r="G260" s="5" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="H260" s="5" t="s">
         <v>16</v>
@@ -12379,12 +12377,12 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="261" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="261" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A261" t="s">
         <v>74</v>
       </c>
       <c r="B261" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C261" s="2">
         <v>1</v>
@@ -12414,7 +12412,7 @@
         <v>20</v>
       </c>
       <c r="M261" s="5" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="O261" s="6">
         <v>43831</v>
@@ -12423,12 +12421,12 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="262" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="262" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A262" t="s">
         <v>74</v>
       </c>
       <c r="B262" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C262" s="2">
         <v>2</v>
@@ -12449,7 +12447,7 @@
         <v>30</v>
       </c>
       <c r="J262" s="5" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="K262" s="5" t="s">
         <v>19</v>
@@ -12467,12 +12465,12 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="263" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="263" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A263" t="s">
         <v>74</v>
       </c>
       <c r="B263" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C263" s="2">
         <v>3</v>
@@ -12510,12 +12508,12 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="264" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="264" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A264" t="s">
         <v>74</v>
       </c>
       <c r="B264" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="C264" s="2">
         <v>4</v>
@@ -12530,7 +12528,7 @@
         <v>97</v>
       </c>
       <c r="G264" s="5" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="H264" t="s">
         <v>16</v>
@@ -12557,12 +12555,12 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="265" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="265" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A265" t="s">
         <v>74</v>
       </c>
       <c r="B265" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C265" s="2">
         <v>1</v>
@@ -12602,24 +12600,24 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="266" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="266" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A266" t="s">
         <v>74</v>
       </c>
       <c r="B266" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C266" s="2">
         <v>2</v>
       </c>
       <c r="D266" s="5" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="E266" s="7" t="s">
         <v>15</v>
       </c>
       <c r="F266" s="5" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="H266" t="s">
         <v>16</v>
@@ -12646,24 +12644,24 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="267" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="267" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A267" t="s">
         <v>74</v>
       </c>
       <c r="B267" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C267" s="2">
         <v>3</v>
       </c>
       <c r="D267" s="5" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="E267" s="8" t="s">
         <v>15</v>
       </c>
       <c r="F267" s="5" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="H267" s="5" t="s">
         <v>19</v>
@@ -12672,7 +12670,7 @@
         <v>20</v>
       </c>
       <c r="J267" s="5" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="K267" s="5" t="s">
         <v>19</v>
@@ -12690,24 +12688,24 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="268" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="268" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A268" t="s">
         <v>74</v>
       </c>
       <c r="B268" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C268" s="2">
         <v>4</v>
       </c>
       <c r="D268" s="5" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E268" s="8" t="s">
         <v>15</v>
       </c>
       <c r="F268" s="5" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="H268" s="5" t="s">
         <v>19</v>
@@ -12734,24 +12732,24 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="269" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="269" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A269" t="s">
         <v>74</v>
       </c>
       <c r="B269" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C269" s="2">
         <v>5</v>
       </c>
       <c r="D269" s="5" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="E269" s="8" t="s">
         <v>15</v>
       </c>
       <c r="F269" s="5" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="H269" s="5" t="s">
         <v>16</v>
@@ -12778,24 +12776,24 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="270" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="270" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A270" t="s">
         <v>74</v>
       </c>
       <c r="B270" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C270" s="2">
         <v>6</v>
       </c>
       <c r="D270" s="5" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="E270" s="8" t="s">
         <v>15</v>
       </c>
       <c r="F270" s="5" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="H270" s="5" t="s">
         <v>16</v>
@@ -12822,12 +12820,12 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="271" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="271" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A271" t="s">
         <v>74</v>
       </c>
       <c r="B271" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C271" s="2">
         <v>7</v>
@@ -12866,12 +12864,12 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="272" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="272" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A272" t="s">
         <v>74</v>
       </c>
       <c r="B272" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C272" s="2">
         <v>8</v>
@@ -12886,7 +12884,7 @@
         <v>97</v>
       </c>
       <c r="G272" s="5" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="H272" s="5" t="s">
         <v>16</v>
@@ -12913,24 +12911,24 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="273" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="273" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A273" t="s">
         <v>74</v>
       </c>
       <c r="B273" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C273" s="2">
         <v>1</v>
       </c>
       <c r="D273" s="5" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="E273" s="8" t="s">
         <v>84</v>
       </c>
       <c r="F273" s="5" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="H273" s="5"/>
       <c r="I273" s="2"/>
@@ -12951,24 +12949,24 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="274" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="274" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A274" t="s">
         <v>74</v>
       </c>
       <c r="B274" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C274" s="2">
         <v>2</v>
       </c>
       <c r="D274" s="5" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="E274" s="7" t="s">
         <v>84</v>
       </c>
       <c r="F274" s="5" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="K274" s="5" t="s">
         <v>19</v>
@@ -12986,24 +12984,24 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="275" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="275" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A275" t="s">
         <v>74</v>
       </c>
       <c r="B275" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C275" s="2">
         <v>3</v>
       </c>
       <c r="D275" s="5" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="E275" s="7" t="s">
         <v>84</v>
       </c>
       <c r="F275" s="5" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="K275" s="5" t="s">
         <v>19</v>
@@ -13021,24 +13019,24 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="276" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="276" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A276" t="s">
         <v>74</v>
       </c>
       <c r="B276" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C276" s="2">
         <v>4</v>
       </c>
       <c r="D276" s="5" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="E276" s="7" t="s">
         <v>84</v>
       </c>
       <c r="F276" s="5" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="K276" s="5" t="s">
         <v>19</v>
@@ -13056,12 +13054,12 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="277" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="277" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A277" t="s">
         <v>74</v>
       </c>
       <c r="B277" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C277" s="2">
         <v>5</v>
@@ -13100,12 +13098,12 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="278" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="278" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A278" t="s">
         <v>74</v>
       </c>
       <c r="B278" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C278" s="2">
         <v>6</v>
@@ -13120,7 +13118,7 @@
         <v>97</v>
       </c>
       <c r="G278" s="5" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="H278" s="5" t="s">
         <v>16</v>
@@ -13147,12 +13145,12 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="279" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="279" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A279" t="s">
         <v>74</v>
       </c>
       <c r="B279" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C279" s="2">
         <v>1</v>
@@ -13191,12 +13189,12 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="280" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="280" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A280" t="s">
         <v>74</v>
       </c>
       <c r="B280" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C280" s="2">
         <v>2</v>
@@ -13226,12 +13224,12 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="281" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="281" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A281" t="s">
         <v>74</v>
       </c>
       <c r="B281" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C281" s="2">
         <v>3</v>
@@ -13261,24 +13259,24 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="282" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="282" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A282" t="s">
         <v>74</v>
       </c>
       <c r="B282" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C282" s="2">
         <v>4</v>
       </c>
       <c r="D282" s="5" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="E282" s="12" t="s">
         <v>84</v>
       </c>
       <c r="F282" s="5" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="K282" s="5" t="s">
         <v>19</v>
@@ -13296,24 +13294,24 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="283" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="283" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A283" t="s">
         <v>74</v>
       </c>
       <c r="B283" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C283" s="2">
         <v>5</v>
       </c>
       <c r="D283" s="5" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="E283" s="12" t="s">
         <v>84</v>
       </c>
       <c r="F283" s="5" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="K283" s="5" t="s">
         <v>19</v>
@@ -13331,24 +13329,24 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="284" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="284" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A284" t="s">
         <v>74</v>
       </c>
       <c r="B284" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C284" s="2">
         <v>6</v>
       </c>
       <c r="D284" s="5" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E284" s="12" t="s">
         <v>84</v>
       </c>
       <c r="F284" s="5" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="K284" s="5" t="s">
         <v>19</v>
@@ -13366,24 +13364,24 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="285" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="285" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A285" t="s">
         <v>74</v>
       </c>
       <c r="B285" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C285" s="2">
         <v>7</v>
       </c>
       <c r="D285" s="5" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E285" s="12" t="s">
         <v>84</v>
       </c>
       <c r="F285" s="5" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="K285" s="5" t="s">
         <v>19</v>
@@ -13401,24 +13399,24 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="286" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="286" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A286" t="s">
         <v>74</v>
       </c>
       <c r="B286" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C286" s="2">
         <v>8</v>
       </c>
       <c r="D286" s="5" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E286" s="12" t="s">
         <v>84</v>
       </c>
       <c r="F286" s="5" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="K286" s="5" t="s">
         <v>19</v>
@@ -13436,24 +13434,24 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="287" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="287" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A287" t="s">
         <v>74</v>
       </c>
       <c r="B287" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C287" s="2">
         <v>9</v>
       </c>
       <c r="D287" s="5" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E287" s="12" t="s">
         <v>84</v>
       </c>
       <c r="F287" s="5" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="K287" s="5" t="s">
         <v>16</v>
@@ -13471,24 +13469,24 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="288" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="288" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A288" t="s">
         <v>74</v>
       </c>
       <c r="B288" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C288" s="2">
         <v>10</v>
       </c>
       <c r="D288" s="5" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E288" s="12" t="s">
         <v>84</v>
       </c>
       <c r="F288" s="5" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="K288" s="5" t="s">
         <v>16</v>
@@ -13497,7 +13495,7 @@
         <v>8</v>
       </c>
       <c r="M288" s="5" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="O288" s="6">
         <v>43831</v>
@@ -13506,24 +13504,24 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="289" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="289" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A289" t="s">
         <v>74</v>
       </c>
       <c r="B289" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C289" s="2">
         <v>11</v>
       </c>
       <c r="D289" s="5" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="E289" s="12" t="s">
         <v>84</v>
       </c>
       <c r="F289" s="5" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="K289" s="5" t="s">
         <v>16</v>
@@ -13541,12 +13539,12 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="290" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="290" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A290" t="s">
         <v>74</v>
       </c>
       <c r="B290" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C290" s="2">
         <v>12</v>
@@ -13576,12 +13574,12 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="291" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="291" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A291" t="s">
         <v>74</v>
       </c>
       <c r="B291" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C291" s="2">
         <v>13</v>
@@ -13596,7 +13594,7 @@
         <v>97</v>
       </c>
       <c r="G291" s="5" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="H291" s="5" t="s">
         <v>16</v>
@@ -13614,12 +13612,12 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="292" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="292" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A292" t="s">
         <v>74</v>
       </c>
       <c r="B292" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C292" s="2">
         <v>1</v>
@@ -13652,24 +13650,24 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="293" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="293" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A293" t="s">
         <v>74</v>
       </c>
       <c r="B293" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C293" s="2">
         <v>2</v>
       </c>
       <c r="D293" s="5" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E293" s="12" t="s">
         <v>84</v>
       </c>
       <c r="F293" s="5" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="K293" t="s">
         <v>19</v>
@@ -13678,7 +13676,7 @@
         <v>255</v>
       </c>
       <c r="M293" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="O293" s="6">
         <v>43831</v>
@@ -13687,24 +13685,24 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="294" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="294" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A294" t="s">
         <v>74</v>
       </c>
       <c r="B294" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C294" s="2">
         <v>3</v>
       </c>
       <c r="D294" s="5" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E294" s="12" t="s">
         <v>84</v>
       </c>
       <c r="F294" s="5" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="K294" t="s">
         <v>19</v>
@@ -13722,12 +13720,12 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="295" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="295" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A295" t="s">
         <v>74</v>
       </c>
       <c r="B295" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C295" s="2">
         <v>4</v>
@@ -13757,12 +13755,12 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="296" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="296" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A296" t="s">
         <v>74</v>
       </c>
       <c r="B296" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C296" s="2">
         <v>5</v>
@@ -13777,7 +13775,7 @@
         <v>97</v>
       </c>
       <c r="G296" s="5" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="H296" s="5" t="s">
         <v>16</v>
@@ -13795,24 +13793,24 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="297" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="297" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A297" t="s">
         <v>74</v>
       </c>
       <c r="B297" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C297" s="2">
         <v>1</v>
       </c>
       <c r="D297" s="5" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="E297" s="12" t="s">
         <v>15</v>
       </c>
       <c r="F297" s="5" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="H297" s="5" t="s">
         <v>19</v>
@@ -13839,18 +13837,18 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="298" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="298" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A298" t="s">
         <v>74</v>
       </c>
       <c r="B298" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C298" s="2">
         <v>2</v>
       </c>
       <c r="D298" s="5" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="E298" s="12" t="s">
         <v>84</v>
@@ -13878,12 +13876,12 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="299" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="299" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A299" t="s">
         <v>74</v>
       </c>
       <c r="B299" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C299" s="2">
         <v>3</v>
@@ -13923,12 +13921,12 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="300" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="300" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A300" t="s">
         <v>74</v>
       </c>
       <c r="B300" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C300" s="2">
         <v>4</v>
@@ -13968,18 +13966,18 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="301" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="301" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A301" t="s">
         <v>74</v>
       </c>
       <c r="B301" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C301" s="2">
         <v>5</v>
       </c>
       <c r="D301" s="5" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="E301" s="12" t="s">
         <v>84</v>
@@ -14007,18 +14005,18 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="302" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="302" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A302" t="s">
         <v>74</v>
       </c>
       <c r="B302" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C302" s="2">
         <v>6</v>
       </c>
       <c r="D302" s="5" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="E302" s="12" t="s">
         <v>84</v>
@@ -14046,18 +14044,18 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="303" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="303" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A303" t="s">
         <v>74</v>
       </c>
       <c r="B303" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C303" s="2">
         <v>7</v>
       </c>
       <c r="D303" s="5" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="E303" s="12" t="s">
         <v>84</v>
@@ -14085,27 +14083,27 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="304" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="304" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A304" t="s">
         <v>74</v>
       </c>
       <c r="B304" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C304" s="2">
         <v>8</v>
       </c>
       <c r="D304" s="5" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="E304" s="12" t="s">
         <v>84</v>
       </c>
       <c r="F304" s="5" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="G304" s="5" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="H304" s="5"/>
       <c r="I304" s="2"/>
@@ -14126,27 +14124,27 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="305" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="305" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A305" t="s">
         <v>74</v>
       </c>
       <c r="B305" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C305" s="2">
         <v>9</v>
       </c>
       <c r="D305" s="5" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="E305" s="12" t="s">
         <v>84</v>
       </c>
       <c r="F305" s="13" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="G305" s="5" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="H305" s="5"/>
       <c r="I305" s="2"/>
@@ -14167,24 +14165,24 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="306" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="306" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A306" t="s">
         <v>74</v>
       </c>
       <c r="B306" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C306" s="2">
         <v>10</v>
       </c>
       <c r="D306" s="5" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="E306" s="12" t="s">
         <v>84</v>
       </c>
       <c r="F306" s="5" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="H306" s="5"/>
       <c r="I306" s="2"/>
@@ -14205,24 +14203,24 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="307" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="307" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A307" t="s">
         <v>74</v>
       </c>
       <c r="B307" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C307" s="2">
         <v>11</v>
       </c>
       <c r="D307" s="5" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E307" s="12" t="s">
         <v>84</v>
       </c>
       <c r="F307" s="5" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="H307" s="5"/>
       <c r="I307" s="2"/>
@@ -14243,27 +14241,27 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="308" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="308" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A308" t="s">
         <v>74</v>
       </c>
       <c r="B308" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C308" s="2">
         <v>12</v>
       </c>
       <c r="D308" s="5" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="E308" s="12" t="s">
         <v>84</v>
       </c>
       <c r="F308" s="5" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="G308" s="5" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="H308" s="5"/>
       <c r="I308" s="2"/>
@@ -14284,27 +14282,27 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="309" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="309" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A309" t="s">
         <v>74</v>
       </c>
       <c r="B309" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C309" s="2">
         <v>13</v>
       </c>
       <c r="D309" s="5" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="E309" s="12" t="s">
         <v>84</v>
       </c>
       <c r="F309" s="5" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="G309" s="5" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="H309" s="5"/>
       <c r="I309" s="2"/>
@@ -14325,18 +14323,18 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="310" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="310" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A310" t="s">
         <v>74</v>
       </c>
       <c r="B310" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C310" s="2">
         <v>14</v>
       </c>
       <c r="D310" s="5" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="E310" s="12" t="s">
         <v>84</v>
@@ -14364,18 +14362,18 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="311" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="311" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A311" t="s">
         <v>74</v>
       </c>
       <c r="B311" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C311" s="2">
         <v>15</v>
       </c>
       <c r="D311" s="5" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="E311" s="12" t="s">
         <v>84</v>
@@ -14403,18 +14401,18 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="312" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="312" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A312" t="s">
         <v>74</v>
       </c>
       <c r="B312" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C312" s="2">
         <v>16</v>
       </c>
       <c r="D312" s="5" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="E312" s="12" t="s">
         <v>84</v>
@@ -14442,18 +14440,18 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="313" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="313" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A313" t="s">
         <v>74</v>
       </c>
       <c r="B313" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C313" s="2">
         <v>17</v>
       </c>
       <c r="D313" s="5" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="E313" s="12" t="s">
         <v>84</v>
@@ -14481,18 +14479,18 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="314" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="314" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A314" t="s">
         <v>74</v>
       </c>
       <c r="B314" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C314" s="2">
         <v>18</v>
       </c>
       <c r="D314" s="5" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="E314" s="12" t="s">
         <v>84</v>
@@ -14520,18 +14518,18 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="315" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="315" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A315" t="s">
         <v>74</v>
       </c>
       <c r="B315" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C315" s="2">
         <v>19</v>
       </c>
       <c r="D315" s="5" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E315" s="12" t="s">
         <v>84</v>
@@ -14559,18 +14557,18 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="316" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="316" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A316" t="s">
         <v>74</v>
       </c>
       <c r="B316" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C316" s="2">
         <v>20</v>
       </c>
       <c r="D316" s="5" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="E316" s="12" t="s">
         <v>84</v>
@@ -14598,18 +14596,18 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="317" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="317" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A317" t="s">
         <v>74</v>
       </c>
       <c r="B317" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C317" s="2">
         <v>21</v>
       </c>
       <c r="D317" s="5" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="E317" s="12" t="s">
         <v>84</v>
@@ -14637,18 +14635,18 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="318" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="318" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A318" t="s">
         <v>74</v>
       </c>
       <c r="B318" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C318" s="2">
         <v>22</v>
       </c>
       <c r="D318" s="5" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="E318" s="12" t="s">
         <v>84</v>
@@ -14676,18 +14674,18 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="319" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="319" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A319" t="s">
         <v>74</v>
       </c>
       <c r="B319" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C319" s="2">
         <v>23</v>
       </c>
       <c r="D319" s="5" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="E319" s="12" t="s">
         <v>84</v>
@@ -14706,7 +14704,7 @@
         <v>8</v>
       </c>
       <c r="M319" s="5" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="O319" s="6">
         <v>43831</v>
@@ -14715,12 +14713,12 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="320" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="320" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A320" t="s">
         <v>74</v>
       </c>
       <c r="B320" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C320" s="2">
         <v>24</v>
@@ -14742,7 +14740,7 @@
         <v>40</v>
       </c>
       <c r="J320" s="5" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="K320" s="5" t="s">
         <v>19</v>
@@ -14751,7 +14749,7 @@
         <v>40</v>
       </c>
       <c r="M320" s="5" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="O320" s="6">
         <v>43831</v>
@@ -14760,18 +14758,18 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="321" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="321" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A321" t="s">
         <v>74</v>
       </c>
       <c r="B321" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C321" s="2">
         <v>25</v>
       </c>
       <c r="D321" s="5" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="E321" s="12" t="s">
         <v>84</v>
@@ -14799,18 +14797,18 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="322" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="322" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A322" t="s">
         <v>74</v>
       </c>
       <c r="B322" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C322" s="2">
         <v>26</v>
       </c>
       <c r="D322" s="5" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="E322" s="12" t="s">
         <v>84</v>
@@ -14838,18 +14836,18 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="323" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="323" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A323" t="s">
         <v>74</v>
       </c>
       <c r="B323" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C323" s="2">
         <v>27</v>
       </c>
       <c r="D323" s="5" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="E323" s="12" t="s">
         <v>84</v>
@@ -14877,18 +14875,18 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="324" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="324" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A324" t="s">
         <v>74</v>
       </c>
       <c r="B324" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C324" s="2">
         <v>28</v>
       </c>
       <c r="D324" s="5" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="E324" s="12" t="s">
         <v>84</v>
@@ -14907,7 +14905,7 @@
         <v>8</v>
       </c>
       <c r="M324" s="5" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="O324" s="6">
         <v>43831</v>
@@ -14916,18 +14914,18 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="325" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="325" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A325" t="s">
         <v>74</v>
       </c>
       <c r="B325" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C325" s="2">
         <v>29</v>
       </c>
       <c r="D325" s="5" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="E325" s="12" t="s">
         <v>84</v>
@@ -14946,7 +14944,7 @@
         <v>8</v>
       </c>
       <c r="M325" s="5" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="O325" s="6">
         <v>43831</v>
@@ -14955,18 +14953,18 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="326" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="326" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A326" t="s">
         <v>74</v>
       </c>
       <c r="B326" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C326" s="2">
         <v>30</v>
       </c>
       <c r="D326" s="5" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="E326" s="12" t="s">
         <v>84</v>
@@ -14985,7 +14983,7 @@
         <v>8</v>
       </c>
       <c r="M326" s="5" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="O326" s="6">
         <v>43831</v>
@@ -14994,18 +14992,18 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="327" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="327" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A327" t="s">
         <v>74</v>
       </c>
       <c r="B327" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C327" s="2">
         <v>31</v>
       </c>
       <c r="D327" s="5" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="E327" s="12" t="s">
         <v>84</v>
@@ -15024,7 +15022,7 @@
         <v>8</v>
       </c>
       <c r="M327" s="5" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="O327" s="6">
         <v>43831</v>
@@ -15033,18 +15031,18 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="328" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="328" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A328" t="s">
         <v>74</v>
       </c>
       <c r="B328" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C328" s="2">
         <v>32</v>
       </c>
       <c r="D328" s="5" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="E328" s="12" t="s">
         <v>84</v>
@@ -15063,7 +15061,7 @@
         <v>8</v>
       </c>
       <c r="M328" s="5" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="O328" s="6">
         <v>43831</v>
@@ -15072,18 +15070,18 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="329" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="329" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A329" t="s">
         <v>74</v>
       </c>
       <c r="B329" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C329" s="2">
         <v>33</v>
       </c>
       <c r="D329" s="5" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="E329" s="12" t="s">
         <v>84</v>
@@ -15102,7 +15100,7 @@
         <v>8</v>
       </c>
       <c r="M329" s="5" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="O329" s="6">
         <v>43831</v>
@@ -15111,18 +15109,18 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="330" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="330" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A330" t="s">
         <v>74</v>
       </c>
       <c r="B330" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C330" s="2">
         <v>34</v>
       </c>
       <c r="D330" s="5" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="E330" s="12" t="s">
         <v>84</v>
@@ -15141,7 +15139,7 @@
         <v>8</v>
       </c>
       <c r="M330" s="5" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="O330" s="6">
         <v>43831</v>
@@ -15150,18 +15148,18 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="331" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="331" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A331" t="s">
         <v>74</v>
       </c>
       <c r="B331" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C331" s="2">
         <v>35</v>
       </c>
       <c r="D331" s="5" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="E331" s="12" t="s">
         <v>84</v>
@@ -15189,18 +15187,18 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="332" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="332" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A332" t="s">
         <v>74</v>
       </c>
       <c r="B332" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C332" s="2">
         <v>36</v>
       </c>
       <c r="D332" s="5" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="E332" s="12" t="s">
         <v>84</v>
@@ -15228,12 +15226,12 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="333" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="333" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A333" t="s">
         <v>74</v>
       </c>
       <c r="B333" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C333" s="2">
         <v>37</v>
@@ -15272,12 +15270,12 @@
         <v>401768</v>
       </c>
     </row>
-    <row r="334" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="334" spans="1:16" hidden="1" x14ac:dyDescent="0.35">
       <c r="A334" t="s">
         <v>74</v>
       </c>
       <c r="B334" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C334" s="2">
         <v>38</v>
@@ -15292,7 +15290,7 @@
         <v>97</v>
       </c>
       <c r="G334" s="5" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="H334" s="1" t="s">
         <v>16</v>
@@ -15320,7 +15318,13 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:Q334"/>
+  <autoFilter ref="A1:Q334">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="FGC_TE_ASTE"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>